<commit_message>
Export excel overall sale actual.
</commit_message>
<xml_diff>
--- a/Sale_Report/Sale_Report/Template/Template-Sale-Report.xlsx
+++ b/Sale_Report/Sale_Report/Template/Template-Sale-Report.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chollatitd\Desktop\Sale Report\Report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Chollatit\_Project\Sale_Report\Sale_Report\Sale_Report\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,6 @@
     <sheet name="12.PMSP Forecast Acc." sheetId="14" r:id="rId12"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -613,16 +612,16 @@
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"_);_(@_)</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>198</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>194</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>235</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>252</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -738,16 +737,16 @@
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"_);_(@_)</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>44</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>38</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>69</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>52</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -863,16 +862,16 @@
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"_);_(@_)</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1006,16 +1005,16 @@
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"_);_(@_)</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>248</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>239</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>311</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>311</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1081,16 +1080,16 @@
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"_);_(@_)</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>238</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>238</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>269</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>269</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1610,7 +1609,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2749,7 +2747,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -3307,7 +3304,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -12271,7 +12267,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -12491,7 +12486,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -12690,7 +12684,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -13295,7 +13288,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -20585,7 +20577,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20627,16 +20619,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="7">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C3" s="7">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D3" s="7">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E3" s="7">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -20644,16 +20636,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="7">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="C4" s="7">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="D4" s="7">
-        <v>69</v>
+        <v>0</v>
       </c>
       <c r="E4" s="7">
-        <v>52</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -20661,16 +20653,16 @@
         <v>3</v>
       </c>
       <c r="B5" s="7">
-        <v>198</v>
+        <v>0</v>
       </c>
       <c r="C5" s="7">
-        <v>194</v>
+        <v>0</v>
       </c>
       <c r="D5" s="7">
-        <v>235</v>
+        <v>0</v>
       </c>
       <c r="E5" s="7">
-        <v>252</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -20679,19 +20671,19 @@
       </c>
       <c r="B6" s="7">
         <f>SUM(B3:B5)</f>
-        <v>248</v>
+        <v>0</v>
       </c>
       <c r="C6" s="7">
         <f t="shared" ref="C6:E6" si="0">SUM(C3:C5)</f>
-        <v>239</v>
+        <v>0</v>
       </c>
       <c r="D6" s="7">
         <f t="shared" si="0"/>
-        <v>311</v>
+        <v>0</v>
       </c>
       <c r="E6" s="7">
         <f t="shared" si="0"/>
-        <v>311</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -20699,16 +20691,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="7">
-        <v>238</v>
+        <v>0</v>
       </c>
       <c r="C7" s="7">
-        <v>238</v>
+        <v>0</v>
       </c>
       <c r="D7" s="7">
-        <v>269</v>
+        <v>0</v>
       </c>
       <c r="E7" s="7">
-        <v>269</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Complete Beta V. 0.8.0
</commit_message>
<xml_diff>
--- a/Sale_Report/Sale_Report/Template/Template-Sale-Report.xlsx
+++ b/Sale_Report/Sale_Report/Template/Template-Sale-Report.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10905" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10905" firstSheet="9" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="1.Overall Monthly sales result" sheetId="1" r:id="rId1"/>
@@ -1605,6 +1605,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1650,16 +1651,16 @@
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"_);_(@_)</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>3306</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1365</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1441</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2180,13 +2181,13 @@
                 <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -2273,16 +2274,16 @@
                 <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2531</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1061</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1089</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2366,16 +2367,16 @@
                 <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>157</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>54</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>62</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2459,16 +2460,16 @@
                 <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2552,16 +2553,16 @@
                 <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.04</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.04</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2646,16 +2647,16 @@
                 <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>76</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>33</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>34</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2743,6 +2744,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2788,16 +2790,16 @@
                 <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2772.1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1152.04</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1187.04</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3300,6 +3302,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -3345,16 +3348,16 @@
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"_);_(@_)</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>533</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>214</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>253</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7647,6 +7650,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -7939,6 +7943,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8233,7 +8238,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -8525,7 +8529,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8801,22 +8804,22 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>289</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>313</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>293</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>286</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>51</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>52</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -8963,28 +8966,28 @@
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"_);_(@_)</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>248</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>310</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>314</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>304</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>295</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>298</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>53</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>53</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -9107,10 +9110,10 @@
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"_);_(@_)</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>238</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>312</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -9243,40 +9246,40 @@
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"_);_(@_)</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>238</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>269</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>291</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>282</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>286</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>296</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>288</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>291</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>265</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>267</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>253</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>281</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10101,43 +10104,43 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>187.85</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>183.19</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>226.18</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>222.72</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>240.41</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>250.24</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>239.73</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>219.87</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>229.85</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>211.42</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>223.99</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
@@ -10146,7 +10149,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>222.67</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>0</c:v>
@@ -10302,43 +10305,43 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.6999999999999993</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.02</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11.69</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11.69</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11.51</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>16.66</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>16.66</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>15.69</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>15.69</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
@@ -10347,7 +10350,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>16.13</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>0</c:v>
@@ -10503,43 +10506,43 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.33</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.33</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.39</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.39</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.44</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.44</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.47</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.45</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.53</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.56000000000000005</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
@@ -10548,7 +10551,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.32</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>0</c:v>
@@ -10704,31 +10707,31 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.01</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.01</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.01</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.01</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.01</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.01</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.01</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.01</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
@@ -10737,10 +10740,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.01</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.01</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
@@ -10749,7 +10752,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.01</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>0</c:v>
@@ -10906,43 +10909,43 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.32</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.59</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.59</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.71</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.74</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.5299999999999998</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8.24</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7.41</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6.19</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6.05</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
@@ -10951,7 +10954,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>7.37</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>0</c:v>
@@ -11244,6 +11247,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -11356,43 +11360,43 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>204.20999999999998</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>200.14</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>243.86</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>241.51999999999998</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>259.07</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>265.89</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>251.31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>245.25</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>254.37</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>233.83999999999997</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>246.3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
@@ -11401,7 +11405,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>246.5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>0</c:v>
@@ -11534,58 +11538,58 @@
                 <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>205</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>205</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>205</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>225</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>225</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>225</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>245</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>245</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>245</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>238</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>238</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>238</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>239</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>239</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>239</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>249</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>249</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>249</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12003,6 +12007,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -12265,6 +12270,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -12337,22 +12343,22 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>45.51</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>47.56</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>47.39</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>52.05</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50.63</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>52.21</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -12484,6 +12490,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -12553,28 +12560,28 @@
                 <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>44.26</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>68.66</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>62.8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>49.81</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>49.02</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>51.78</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>53.15</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>53.25</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -12682,6 +12689,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -12751,10 +12759,10 @@
                 <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>37.93</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>51.92</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -12888,40 +12896,40 @@
                 <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>33.61</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43.58</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>45.45</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43.39</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>47.52</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>47.21</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>47.21</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>49.46</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>40.46</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44.93</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43.13</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>47.07</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13286,6 +13294,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -20720,7 +20729,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:E1"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20752,16 +20761,16 @@
         <v>48</v>
       </c>
       <c r="B2" s="7">
-        <v>3306</v>
+        <v>0</v>
       </c>
       <c r="C2" s="7">
         <v>0</v>
       </c>
       <c r="D2" s="7">
-        <v>1365</v>
+        <v>0</v>
       </c>
       <c r="E2" s="7">
-        <v>1441</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -20775,8 +20784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20808,13 +20817,13 @@
         <v>7</v>
       </c>
       <c r="B2" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="8">
         <v>0</v>
       </c>
       <c r="D2" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" s="8">
         <v>0</v>
@@ -20825,16 +20834,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="8">
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="C3" s="8">
         <v>0</v>
       </c>
       <c r="D3" s="8">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="E3" s="8">
-        <v>34</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -20842,16 +20851,16 @@
         <v>8</v>
       </c>
       <c r="B4" s="8">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C4" s="8">
         <v>0</v>
       </c>
       <c r="D4" s="8">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E4" s="8">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -20859,16 +20868,16 @@
         <v>18</v>
       </c>
       <c r="B5" s="8">
-        <v>157</v>
+        <v>0</v>
       </c>
       <c r="C5" s="8">
         <v>0</v>
       </c>
       <c r="D5" s="8">
-        <v>54</v>
+        <v>0</v>
       </c>
       <c r="E5" s="8">
-        <v>62</v>
+        <v>0</v>
       </c>
       <c r="K5" t="s">
         <v>52</v>
@@ -20879,16 +20888,16 @@
         <v>3</v>
       </c>
       <c r="B6" s="8">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="8">
         <v>0</v>
       </c>
       <c r="D6" s="8">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="E6" s="8">
-        <v>0.04</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -20896,16 +20905,16 @@
         <v>10</v>
       </c>
       <c r="B7" s="8">
-        <v>2531</v>
+        <v>0</v>
       </c>
       <c r="C7" s="8">
         <v>0</v>
       </c>
       <c r="D7" s="8">
-        <v>1061</v>
+        <v>0</v>
       </c>
       <c r="E7" s="8">
-        <v>1089</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -20931,7 +20940,7 @@
       </c>
       <c r="B9" s="8">
         <f>SUM(B2:B8)</f>
-        <v>2772.1</v>
+        <v>0</v>
       </c>
       <c r="C9" s="8">
         <f t="shared" ref="C9:E9" si="0">SUM(C2:C8)</f>
@@ -20939,11 +20948,11 @@
       </c>
       <c r="D9" s="8">
         <f t="shared" si="0"/>
-        <v>1152.04</v>
+        <v>0</v>
       </c>
       <c r="E9" s="8">
         <f t="shared" si="0"/>
-        <v>1187.04</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -20957,8 +20966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20990,16 +20999,16 @@
         <v>2</v>
       </c>
       <c r="B2" s="7">
-        <v>533</v>
+        <v>0</v>
       </c>
       <c r="C2" s="7">
         <v>0</v>
       </c>
       <c r="D2" s="7">
-        <v>214</v>
+        <v>0</v>
       </c>
       <c r="E2" s="7">
-        <v>253</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -21623,7 +21632,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
@@ -21679,8 +21688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21736,22 +21745,22 @@
         <v>0</v>
       </c>
       <c r="C2" s="7">
-        <v>289</v>
+        <v>0</v>
       </c>
       <c r="D2" s="7">
-        <v>313</v>
+        <v>0</v>
       </c>
       <c r="E2" s="7">
-        <v>293</v>
+        <v>0</v>
       </c>
       <c r="F2" s="7">
-        <v>286</v>
+        <v>0</v>
       </c>
       <c r="G2" s="7">
-        <v>51</v>
+        <v>0</v>
       </c>
       <c r="H2" s="7">
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="I2" s="7">
         <v>0</v>
@@ -21774,28 +21783,28 @@
         <v>38</v>
       </c>
       <c r="B3" s="7">
-        <v>248</v>
+        <v>0</v>
       </c>
       <c r="C3" s="7">
-        <v>310</v>
+        <v>0</v>
       </c>
       <c r="D3" s="7">
-        <v>314</v>
+        <v>0</v>
       </c>
       <c r="E3" s="7">
-        <v>304</v>
+        <v>0</v>
       </c>
       <c r="F3" s="7">
-        <v>295</v>
+        <v>0</v>
       </c>
       <c r="G3" s="7">
-        <v>298</v>
+        <v>0</v>
       </c>
       <c r="H3" s="7">
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="I3" s="7">
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="J3" s="7">
         <v>0</v>
@@ -21815,10 +21824,10 @@
         <v>6</v>
       </c>
       <c r="B4" s="7">
-        <v>238</v>
+        <v>0</v>
       </c>
       <c r="C4" s="7">
-        <v>312</v>
+        <v>0</v>
       </c>
       <c r="D4" s="7">
         <v>0</v>
@@ -21856,40 +21865,40 @@
         <v>39</v>
       </c>
       <c r="B5" s="7">
-        <v>238</v>
+        <v>0</v>
       </c>
       <c r="C5" s="7">
-        <v>269</v>
+        <v>0</v>
       </c>
       <c r="D5" s="7">
-        <v>291</v>
+        <v>0</v>
       </c>
       <c r="E5" s="7">
-        <v>282</v>
+        <v>0</v>
       </c>
       <c r="F5" s="7">
-        <v>286</v>
+        <v>0</v>
       </c>
       <c r="G5" s="7">
-        <v>296</v>
+        <v>0</v>
       </c>
       <c r="H5" s="7">
-        <v>288</v>
+        <v>0</v>
       </c>
       <c r="I5" s="7">
-        <v>291</v>
+        <v>0</v>
       </c>
       <c r="J5" s="7">
-        <v>265</v>
+        <v>0</v>
       </c>
       <c r="K5" s="7">
-        <v>267</v>
+        <v>0</v>
       </c>
       <c r="L5" s="7">
-        <v>253</v>
+        <v>0</v>
       </c>
       <c r="M5" s="7">
-        <v>281</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -21944,8 +21953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S12"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22111,43 +22120,43 @@
         <v>0</v>
       </c>
       <c r="C4" s="8">
-        <v>6.32</v>
+        <v>0</v>
       </c>
       <c r="D4" s="8">
-        <v>6.59</v>
+        <v>0</v>
       </c>
       <c r="E4" s="8">
-        <v>5.59</v>
+        <v>0</v>
       </c>
       <c r="F4" s="8">
-        <v>6.71</v>
+        <v>0</v>
       </c>
       <c r="G4" s="9">
-        <v>6.74</v>
+        <v>0</v>
       </c>
       <c r="H4" s="8">
-        <v>6.6</v>
+        <v>0</v>
       </c>
       <c r="I4" s="8">
-        <v>2.5299999999999998</v>
+        <v>0</v>
       </c>
       <c r="J4" s="8">
         <v>0</v>
       </c>
       <c r="K4" s="8">
-        <v>8.24</v>
+        <v>0</v>
       </c>
       <c r="L4" s="8">
-        <v>7.41</v>
+        <v>0</v>
       </c>
       <c r="M4" s="8">
         <v>0</v>
       </c>
       <c r="N4" s="8">
-        <v>6.19</v>
+        <v>0</v>
       </c>
       <c r="O4" s="8">
-        <v>6.05</v>
+        <v>0</v>
       </c>
       <c r="P4" s="8">
         <v>0</v>
@@ -22156,7 +22165,7 @@
         <v>0</v>
       </c>
       <c r="R4" s="8">
-        <v>7.37</v>
+        <v>0</v>
       </c>
       <c r="S4" s="8">
         <v>0</v>
@@ -22170,31 +22179,31 @@
         <v>0</v>
       </c>
       <c r="C5" s="8">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="D5" s="8">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="E5" s="8">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="F5" s="8">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="G5" s="8">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="H5" s="8">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="I5" s="8">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="J5" s="8">
         <v>0</v>
       </c>
       <c r="K5" s="8">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="L5" s="8">
         <v>0</v>
@@ -22203,10 +22212,10 @@
         <v>0</v>
       </c>
       <c r="N5" s="8">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="O5" s="8">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="P5" s="8">
         <v>0</v>
@@ -22215,7 +22224,7 @@
         <v>0</v>
       </c>
       <c r="R5" s="8">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="S5" s="8">
         <v>0</v>
@@ -22229,43 +22238,43 @@
         <v>0</v>
       </c>
       <c r="C6" s="8">
-        <v>0.33</v>
+        <v>0</v>
       </c>
       <c r="D6" s="8">
-        <v>0.33</v>
+        <v>0</v>
       </c>
       <c r="E6" s="8">
-        <v>0.39</v>
+        <v>0</v>
       </c>
       <c r="F6" s="8">
-        <v>0.39</v>
+        <v>0</v>
       </c>
       <c r="G6" s="8">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="H6" s="8">
-        <v>0.44</v>
+        <v>0</v>
       </c>
       <c r="I6" s="8">
-        <v>0.44</v>
+        <v>0</v>
       </c>
       <c r="J6" s="8">
         <v>0</v>
       </c>
       <c r="K6" s="8">
-        <v>0.47</v>
+        <v>0</v>
       </c>
       <c r="L6" s="8">
-        <v>0.45</v>
+        <v>0</v>
       </c>
       <c r="M6" s="8">
         <v>0</v>
       </c>
       <c r="N6" s="8">
-        <v>0.53</v>
+        <v>0</v>
       </c>
       <c r="O6" s="8">
-        <v>0.56000000000000005</v>
+        <v>0</v>
       </c>
       <c r="P6" s="8">
         <v>0</v>
@@ -22274,7 +22283,7 @@
         <v>0</v>
       </c>
       <c r="R6" s="8">
-        <v>0.32</v>
+        <v>0</v>
       </c>
       <c r="S6" s="8">
         <v>0</v>
@@ -22288,43 +22297,43 @@
         <v>0</v>
       </c>
       <c r="C7" s="8">
-        <v>9.6999999999999993</v>
+        <v>0</v>
       </c>
       <c r="D7" s="8">
-        <v>10.02</v>
+        <v>0</v>
       </c>
       <c r="E7" s="8">
-        <v>11.69</v>
+        <v>0</v>
       </c>
       <c r="F7" s="8">
-        <v>11.69</v>
+        <v>0</v>
       </c>
       <c r="G7" s="8">
-        <v>11.51</v>
+        <v>0</v>
       </c>
       <c r="H7" s="8">
-        <v>8.6</v>
+        <v>0</v>
       </c>
       <c r="I7" s="8">
-        <v>8.6</v>
+        <v>0</v>
       </c>
       <c r="J7" s="8">
         <v>0</v>
       </c>
       <c r="K7" s="8">
-        <v>16.66</v>
+        <v>0</v>
       </c>
       <c r="L7" s="8">
-        <v>16.66</v>
+        <v>0</v>
       </c>
       <c r="M7" s="8">
         <v>0</v>
       </c>
       <c r="N7" s="8">
-        <v>15.69</v>
+        <v>0</v>
       </c>
       <c r="O7" s="8">
-        <v>15.69</v>
+        <v>0</v>
       </c>
       <c r="P7" s="8">
         <v>0</v>
@@ -22333,7 +22342,7 @@
         <v>0</v>
       </c>
       <c r="R7" s="8">
-        <v>16.13</v>
+        <v>0</v>
       </c>
       <c r="S7" s="8">
         <v>0</v>
@@ -22347,43 +22356,43 @@
         <v>0</v>
       </c>
       <c r="C8" s="8">
-        <v>187.85</v>
+        <v>0</v>
       </c>
       <c r="D8" s="8">
-        <v>183.19</v>
+        <v>0</v>
       </c>
       <c r="E8" s="8">
-        <v>226.18</v>
+        <v>0</v>
       </c>
       <c r="F8" s="8">
-        <v>222.72</v>
+        <v>0</v>
       </c>
       <c r="G8" s="8">
-        <v>240.41</v>
+        <v>0</v>
       </c>
       <c r="H8" s="8">
-        <v>250.24</v>
+        <v>0</v>
       </c>
       <c r="I8" s="8">
-        <v>239.73</v>
+        <v>0</v>
       </c>
       <c r="J8" s="8">
         <v>0</v>
       </c>
       <c r="K8" s="8">
-        <v>219.87</v>
+        <v>0</v>
       </c>
       <c r="L8" s="8">
-        <v>229.85</v>
+        <v>0</v>
       </c>
       <c r="M8" s="8">
         <v>0</v>
       </c>
       <c r="N8" s="8">
-        <v>211.42</v>
+        <v>0</v>
       </c>
       <c r="O8" s="8">
-        <v>223.99</v>
+        <v>0</v>
       </c>
       <c r="P8" s="8">
         <v>0</v>
@@ -22392,7 +22401,7 @@
         <v>0</v>
       </c>
       <c r="R8" s="8">
-        <v>222.67</v>
+        <v>0</v>
       </c>
       <c r="S8" s="8">
         <v>0</v>
@@ -22467,31 +22476,31 @@
       </c>
       <c r="C10" s="8">
         <f t="shared" ref="C10:S10" si="0">SUM(C3:C9)</f>
-        <v>204.20999999999998</v>
+        <v>0</v>
       </c>
       <c r="D10" s="8">
         <f t="shared" si="0"/>
-        <v>200.14</v>
+        <v>0</v>
       </c>
       <c r="E10" s="8">
         <f t="shared" si="0"/>
-        <v>243.86</v>
+        <v>0</v>
       </c>
       <c r="F10" s="8">
         <f t="shared" si="0"/>
-        <v>241.51999999999998</v>
+        <v>0</v>
       </c>
       <c r="G10" s="8">
         <f t="shared" si="0"/>
-        <v>259.07</v>
+        <v>0</v>
       </c>
       <c r="H10" s="8">
         <f t="shared" si="0"/>
-        <v>265.89</v>
+        <v>0</v>
       </c>
       <c r="I10" s="8">
         <f t="shared" si="0"/>
-        <v>251.31</v>
+        <v>0</v>
       </c>
       <c r="J10" s="8">
         <f t="shared" si="0"/>
@@ -22499,11 +22508,11 @@
       </c>
       <c r="K10" s="8">
         <f t="shared" si="0"/>
-        <v>245.25</v>
+        <v>0</v>
       </c>
       <c r="L10" s="8">
         <f t="shared" si="0"/>
-        <v>254.37</v>
+        <v>0</v>
       </c>
       <c r="M10" s="8">
         <f t="shared" si="0"/>
@@ -22511,11 +22520,11 @@
       </c>
       <c r="N10" s="8">
         <f t="shared" si="0"/>
-        <v>233.83999999999997</v>
+        <v>0</v>
       </c>
       <c r="O10" s="8">
         <f t="shared" si="0"/>
-        <v>246.3</v>
+        <v>0</v>
       </c>
       <c r="P10" s="8">
         <f t="shared" si="0"/>
@@ -22527,7 +22536,7 @@
       </c>
       <c r="R10" s="8">
         <f t="shared" si="0"/>
-        <v>246.5</v>
+        <v>0</v>
       </c>
       <c r="S10" s="8">
         <f t="shared" si="0"/>
@@ -22539,58 +22548,58 @@
         <v>5</v>
       </c>
       <c r="B11" s="8">
-        <v>205</v>
+        <v>0</v>
       </c>
       <c r="C11" s="8">
-        <v>205</v>
+        <v>0</v>
       </c>
       <c r="D11" s="8">
-        <v>205</v>
+        <v>0</v>
       </c>
       <c r="E11" s="8">
-        <v>225</v>
+        <v>0</v>
       </c>
       <c r="F11" s="8">
-        <v>225</v>
+        <v>0</v>
       </c>
       <c r="G11" s="8">
-        <v>225</v>
+        <v>0</v>
       </c>
       <c r="H11" s="8">
-        <v>245</v>
+        <v>0</v>
       </c>
       <c r="I11" s="8">
-        <v>245</v>
+        <v>0</v>
       </c>
       <c r="J11" s="8">
-        <v>245</v>
+        <v>0</v>
       </c>
       <c r="K11" s="8">
-        <v>238</v>
+        <v>0</v>
       </c>
       <c r="L11" s="8">
-        <v>238</v>
+        <v>0</v>
       </c>
       <c r="M11" s="8">
-        <v>238</v>
+        <v>0</v>
       </c>
       <c r="N11" s="8">
-        <v>239</v>
+        <v>0</v>
       </c>
       <c r="O11" s="8">
-        <v>239</v>
+        <v>0</v>
       </c>
       <c r="P11" s="8">
-        <v>239</v>
+        <v>0</v>
       </c>
       <c r="Q11" s="8">
-        <v>249</v>
+        <v>0</v>
       </c>
       <c r="R11" s="8">
-        <v>249</v>
+        <v>0</v>
       </c>
       <c r="S11" s="8">
-        <v>249</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -22672,7 +22681,7 @@
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22728,22 +22737,22 @@
         <v>0</v>
       </c>
       <c r="C2" s="8">
-        <v>45.51</v>
+        <v>0</v>
       </c>
       <c r="D2" s="8">
-        <v>47.56</v>
+        <v>0</v>
       </c>
       <c r="E2" s="8">
-        <v>47.39</v>
+        <v>0</v>
       </c>
       <c r="F2" s="8">
-        <v>52.05</v>
+        <v>0</v>
       </c>
       <c r="G2" s="8">
-        <v>50.63</v>
+        <v>0</v>
       </c>
       <c r="H2" s="8">
-        <v>52.21</v>
+        <v>0</v>
       </c>
       <c r="I2" s="8">
         <v>0</v>
@@ -22766,28 +22775,28 @@
         <v>38</v>
       </c>
       <c r="B3" s="8">
-        <v>44.26</v>
+        <v>0</v>
       </c>
       <c r="C3" s="8">
-        <v>68.66</v>
+        <v>0</v>
       </c>
       <c r="D3" s="8">
-        <v>62.8</v>
+        <v>0</v>
       </c>
       <c r="E3" s="8">
-        <v>49.81</v>
+        <v>0</v>
       </c>
       <c r="F3" s="8">
-        <v>49.02</v>
+        <v>0</v>
       </c>
       <c r="G3" s="8">
-        <v>51.78</v>
+        <v>0</v>
       </c>
       <c r="H3" s="8">
-        <v>53.15</v>
+        <v>0</v>
       </c>
       <c r="I3" s="8">
-        <v>53.25</v>
+        <v>0</v>
       </c>
       <c r="J3" s="8">
         <v>0</v>
@@ -22807,10 +22816,10 @@
         <v>6</v>
       </c>
       <c r="B4" s="8">
-        <v>37.93</v>
+        <v>0</v>
       </c>
       <c r="C4" s="8">
-        <v>51.92</v>
+        <v>0</v>
       </c>
       <c r="D4" s="8">
         <v>0</v>
@@ -22848,40 +22857,40 @@
         <v>46</v>
       </c>
       <c r="B5" s="8">
-        <v>33.61</v>
+        <v>0</v>
       </c>
       <c r="C5" s="8">
-        <v>43.58</v>
+        <v>0</v>
       </c>
       <c r="D5" s="8">
-        <v>45.45</v>
+        <v>0</v>
       </c>
       <c r="E5" s="8">
-        <v>43.39</v>
+        <v>0</v>
       </c>
       <c r="F5" s="8">
-        <v>47.52</v>
+        <v>0</v>
       </c>
       <c r="G5" s="8">
-        <v>47.21</v>
+        <v>0</v>
       </c>
       <c r="H5" s="8">
-        <v>47.21</v>
+        <v>0</v>
       </c>
       <c r="I5" s="8">
-        <v>49.46</v>
+        <v>0</v>
       </c>
       <c r="J5" s="8">
-        <v>40.46</v>
+        <v>0</v>
       </c>
       <c r="K5" s="8">
-        <v>44.93</v>
+        <v>0</v>
       </c>
       <c r="L5" s="8">
-        <v>43.13</v>
+        <v>0</v>
       </c>
       <c r="M5" s="8">
-        <v>47.07</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>